<commit_message>
add scripts for 3 graphs
</commit_message>
<xml_diff>
--- a/pH_optode/data/RWS_01_11.xlsx
+++ b/pH_optode/data/RWS_01_11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_GITHUB/lab-work/pH_optode/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="557" documentId="8_{0985D069-2439-40B4-A76B-47398E5EA00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{81861A1A-EAE1-4E13-9E38-909A4B289FE0}"/>
+  <xr:revisionPtr revIDLastSave="563" documentId="8_{0985D069-2439-40B4-A76B-47398E5EA00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AFFD75D4-E92C-4571-9FCB-282BBD9BDE77}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AFFA04B0-61ED-42A2-921A-E115E7B57E02}"/>
   </bookViews>
@@ -1285,8 +1285,8 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O42" sqref="O42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added graph diff vs ph opt
</commit_message>
<xml_diff>
--- a/pH_optode/data/RWS_01_11.xlsx
+++ b/pH_optode/data/RWS_01_11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_GITHUB/lab-work/pH_optode/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="563" documentId="8_{0985D069-2439-40B4-A76B-47398E5EA00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AFFD75D4-E92C-4571-9FCB-282BBD9BDE77}"/>
+  <xr:revisionPtr revIDLastSave="564" documentId="8_{0985D069-2439-40B4-A76B-47398E5EA00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{567249F9-E0F4-4234-9C20-E9CFA5C038B5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AFFA04B0-61ED-42A2-921A-E115E7B57E02}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AFFA04B0-61ED-42A2-921A-E115E7B57E02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1284,26 +1284,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24354337-39CE-416A-A127-42BEC72437C4}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="10"/>
-    <col min="10" max="10" width="10.7109375" style="20"/>
-    <col min="12" max="12" width="10.7109375" style="29"/>
-    <col min="14" max="14" width="10.7109375" style="11"/>
-    <col min="15" max="15" width="10.7109375" style="29"/>
-    <col min="18" max="18" width="19.42578125" customWidth="1"/>
+    <col min="1" max="2" width="15.26953125" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="10"/>
+    <col min="10" max="10" width="10.7265625" style="20"/>
+    <col min="12" max="12" width="10.7265625" style="29"/>
+    <col min="14" max="14" width="10.7265625" style="11"/>
+    <col min="15" max="15" width="10.7265625" style="29"/>
+    <col min="18" max="18" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>22</v>
       </c>
@@ -1464,7 +1464,7 @@
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
     </row>
-    <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="31">
         <v>44113</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="31">
         <v>44113</v>
       </c>
@@ -1550,7 +1550,7 @@
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
     </row>
-    <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="31">
         <v>44113</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B7" s="31">
         <v>44113</v>
       </c>
@@ -1636,7 +1636,7 @@
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
     </row>
-    <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="31">
         <v>44113</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="31">
         <v>44113</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="31">
         <v>44113</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="31">
         <v>44113</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="31">
         <v>44113</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B13" s="31">
         <v>44113</v>
       </c>
@@ -1891,7 +1891,7 @@
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B14" s="31">
         <v>44113</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B15" s="31">
         <v>44113</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B16" s="31">
         <v>44113</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
         <v>22</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
         <v>22</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="25" t="s">
         <v>50</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B20" s="31" t="s">
         <v>50</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="25" t="s">
         <v>50</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="25" t="s">
         <v>50</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="25" t="s">
         <v>50</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B24" s="25" t="s">
         <v>50</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="25" t="s">
         <v>50</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B26" s="25" t="s">
         <v>50</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B27" s="25" t="s">
         <v>50</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B28" s="25" t="s">
         <v>50</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B29" s="25" t="s">
         <v>50</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B30" s="25" t="s">
         <v>50</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B31" s="25" t="s">
         <v>50</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B32" s="25" t="s">
         <v>50</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B33" s="25" t="s">
         <v>50</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="30" t="s">
         <v>22</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="30" t="s">
         <v>22</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B36" s="31" t="s">
         <v>81</v>
       </c>
@@ -2847,7 +2847,7 @@
       <c r="J36" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="K36" s="30">
+      <c r="K36" s="7">
         <v>7.8</v>
       </c>
       <c r="L36" s="7">
@@ -2860,7 +2860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B37" s="31" t="s">
         <v>81</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B38" s="31" t="s">
         <v>81</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B39" s="31" t="s">
         <v>81</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B40" s="31" t="s">
         <v>81</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B41" s="31" t="s">
         <v>81</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B42" s="31" t="s">
         <v>81</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B43" s="31" t="s">
         <v>81</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B44" s="31" t="s">
         <v>81</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B45" s="31" t="s">
         <v>81</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="30" t="s">
         <v>22</v>
       </c>
@@ -3291,21 +3291,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027E85BF46FFBA5448F68919BA489A1DA" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="45a9c6a0386fdd3966398fc659f672bc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d8e2f2e6-fcba-4c24-ae89-6c4ebe1d1211" xmlns:ns4="1e11a0bb-5c52-4e83-8dd3-aa81c1705742" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5fd16eb0bef241ffc3cb418196d56410" ns3:_="" ns4:_="">
     <xsd:import namespace="d8e2f2e6-fcba-4c24-ae89-6c4ebe1d1211"/>
@@ -3528,24 +3513,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91E16F44-C68D-4E79-A4BA-87CF7924D4A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77FFA200-F0B2-4031-AD08-862C0DB7F006}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46B2F9E1-9454-4E0C-80CD-4240C2750498}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3562,4 +3545,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77FFA200-F0B2-4031-AD08-862C0DB7F006}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91E16F44-C68D-4E79-A4BA-87CF7924D4A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>